<commit_message>
[CONFIG]: Se cambian logicas y estructuras de tablas/relaciones.
</commit_message>
<xml_diff>
--- a/TransferenciasRecibidas.xlsx
+++ b/TransferenciasRecibidas.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63533418-EFEB-471F-AC89-1956DA25B820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D1531D6-7A97-4A82-A5BD-78AAFBD104C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="24220" windowHeight="13000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transferencias Recibidas" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1648" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="758">
   <si>
     <t>Grupo</t>
   </si>
@@ -1206,9 +1206,6 @@
   </si>
   <si>
     <t>061449096630</t>
-  </si>
-  <si>
-    <t>780</t>
   </si>
   <si>
     <t>061538043597</t>
@@ -2426,6 +2423,13 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2434,13 +2438,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2809,8 +2806,8 @@
   </sheetPr>
   <dimension ref="A1:Q154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90:B90"/>
+    <sheetView tabSelected="1" topLeftCell="J59" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -2834,44 +2831,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" customHeight="1">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
@@ -2880,21 +2877,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
@@ -2903,69 +2900,69 @@
         <v>4</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" ht="34" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
     </row>
     <row r="7" spans="1:17" ht="30" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
@@ -3009,10 +3006,10 @@
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
@@ -3054,10 +3051,10 @@
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
@@ -3099,10 +3096,10 @@
       <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="3" t="s">
         <v>44</v>
       </c>
@@ -3144,10 +3141,10 @@
       <c r="Q10" s="2"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="3" t="s">
         <v>44</v>
       </c>
@@ -3189,10 +3186,10 @@
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="3" t="s">
         <v>44</v>
       </c>
@@ -3234,10 +3231,10 @@
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="3" t="s">
         <v>58</v>
       </c>
@@ -3279,10 +3276,10 @@
       <c r="Q13" s="2"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="3" t="s">
         <v>64</v>
       </c>
@@ -3320,10 +3317,10 @@
       <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="3" t="s">
         <v>58</v>
       </c>
@@ -3361,10 +3358,10 @@
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="3" t="s">
         <v>22</v>
       </c>
@@ -3402,10 +3399,10 @@
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="3" t="s">
         <v>58</v>
       </c>
@@ -3443,10 +3440,10 @@
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="3" t="s">
         <v>64</v>
       </c>
@@ -3484,10 +3481,10 @@
       <c r="Q18" s="2"/>
     </row>
     <row r="19" spans="1:17" ht="15" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="3" t="s">
         <v>44</v>
       </c>
@@ -3525,10 +3522,10 @@
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17" ht="15" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
@@ -3566,10 +3563,10 @@
       <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="3" t="s">
         <v>58</v>
       </c>
@@ -3607,10 +3604,10 @@
       <c r="Q21" s="2"/>
     </row>
     <row r="22" spans="1:17" ht="15" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="3" t="s">
         <v>58</v>
       </c>
@@ -3648,10 +3645,10 @@
       <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="3" t="s">
         <v>44</v>
       </c>
@@ -3689,10 +3686,10 @@
       <c r="Q23" s="2"/>
     </row>
     <row r="24" spans="1:17" ht="15" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="3" t="s">
         <v>44</v>
       </c>
@@ -3730,10 +3727,10 @@
       <c r="Q24" s="2"/>
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3" t="s">
         <v>130</v>
       </c>
@@ -3771,10 +3768,10 @@
       <c r="Q25" s="2"/>
     </row>
     <row r="26" spans="1:17" ht="15" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="3" t="s">
         <v>130</v>
       </c>
@@ -3812,10 +3809,10 @@
       <c r="Q26" s="2"/>
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
@@ -3853,10 +3850,10 @@
       <c r="Q27" s="2"/>
     </row>
     <row r="28" spans="1:17" ht="15" customHeight="1">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="3" t="s">
         <v>35</v>
       </c>
@@ -3894,10 +3891,10 @@
       <c r="Q28" s="2"/>
     </row>
     <row r="29" spans="1:17" ht="15" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="3" t="s">
         <v>35</v>
       </c>
@@ -3935,10 +3932,10 @@
       <c r="Q29" s="2"/>
     </row>
     <row r="30" spans="1:17" ht="15" customHeight="1">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="3" t="s">
         <v>22</v>
       </c>
@@ -3976,10 +3973,10 @@
       <c r="Q30" s="2"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
         <v>22</v>
       </c>
@@ -4017,10 +4014,10 @@
       <c r="Q31" s="2"/>
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B32" s="6"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
         <v>22</v>
       </c>
@@ -4058,10 +4055,10 @@
       <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B33" s="6"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="3" t="s">
         <v>64</v>
       </c>
@@ -4099,10 +4096,10 @@
       <c r="Q33" s="2"/>
     </row>
     <row r="34" spans="1:17" ht="15" customHeight="1">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="B34" s="6"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="3" t="s">
         <v>64</v>
       </c>
@@ -4140,10 +4137,10 @@
       <c r="Q34" s="2"/>
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="B35" s="6"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="3" t="s">
         <v>64</v>
       </c>
@@ -4181,10 +4178,10 @@
       <c r="Q35" s="2"/>
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B36" s="6"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="3" t="s">
         <v>64</v>
       </c>
@@ -4222,10 +4219,10 @@
       <c r="Q36" s="2"/>
     </row>
     <row r="37" spans="1:17" ht="15" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B37" s="6"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="3" t="s">
         <v>58</v>
       </c>
@@ -4263,10 +4260,10 @@
       <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="1:17" ht="15" customHeight="1">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="3" t="s">
         <v>58</v>
       </c>
@@ -4304,10 +4301,10 @@
       <c r="Q38" s="2"/>
     </row>
     <row r="39" spans="1:17" ht="15" customHeight="1">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="3" t="s">
         <v>58</v>
       </c>
@@ -4345,10 +4342,10 @@
       <c r="Q39" s="2"/>
     </row>
     <row r="40" spans="1:17" ht="15" customHeight="1">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B40" s="6"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="3" t="s">
         <v>58</v>
       </c>
@@ -4386,10 +4383,10 @@
       <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" ht="15" customHeight="1">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="B41" s="6"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="3" t="s">
         <v>58</v>
       </c>
@@ -4427,10 +4424,10 @@
       <c r="Q41" s="2"/>
     </row>
     <row r="42" spans="1:17" ht="15" customHeight="1">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="B42" s="6"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="3" t="s">
         <v>58</v>
       </c>
@@ -4468,10 +4465,10 @@
       <c r="Q42" s="2"/>
     </row>
     <row r="43" spans="1:17" ht="15" customHeight="1">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B43" s="6"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="3" t="s">
         <v>35</v>
       </c>
@@ -4509,10 +4506,10 @@
       <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="1:17" ht="15" customHeight="1">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="B44" s="6"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
         <v>44</v>
       </c>
@@ -4550,10 +4547,10 @@
       <c r="Q44" s="2"/>
     </row>
     <row r="45" spans="1:17" ht="15" customHeight="1">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="3" t="s">
         <v>44</v>
       </c>
@@ -4591,10 +4588,10 @@
       <c r="Q45" s="2"/>
     </row>
     <row r="46" spans="1:17" ht="15" customHeight="1">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="3" t="s">
         <v>44</v>
       </c>
@@ -4632,10 +4629,10 @@
       <c r="Q46" s="2"/>
     </row>
     <row r="47" spans="1:17" ht="15" customHeight="1">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="3" t="s">
         <v>22</v>
       </c>
@@ -4673,10 +4670,10 @@
       <c r="Q47" s="2"/>
     </row>
     <row r="48" spans="1:17" ht="15" customHeight="1">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B48" s="6"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="3" t="s">
         <v>130</v>
       </c>
@@ -4714,10 +4711,10 @@
       <c r="Q48" s="2"/>
     </row>
     <row r="49" spans="1:17" ht="15" customHeight="1">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="3" t="s">
         <v>130</v>
       </c>
@@ -4755,10 +4752,10 @@
       <c r="Q49" s="2"/>
     </row>
     <row r="50" spans="1:17" ht="15" customHeight="1">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="3" t="s">
         <v>130</v>
       </c>
@@ -4796,10 +4793,10 @@
       <c r="Q50" s="2"/>
     </row>
     <row r="51" spans="1:17" ht="15" customHeight="1">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="3" t="s">
         <v>130</v>
       </c>
@@ -4837,10 +4834,10 @@
       <c r="Q51" s="2"/>
     </row>
     <row r="52" spans="1:17" ht="15" customHeight="1">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="B52" s="6"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="3" t="s">
         <v>268</v>
       </c>
@@ -4878,10 +4875,10 @@
       <c r="Q52" s="2"/>
     </row>
     <row r="53" spans="1:17" ht="15" customHeight="1">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B53" s="6"/>
+      <c r="B53" s="8"/>
       <c r="C53" s="3" t="s">
         <v>35</v>
       </c>
@@ -4919,10 +4916,10 @@
       <c r="Q53" s="2"/>
     </row>
     <row r="54" spans="1:17" ht="15" customHeight="1">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="B54" s="6"/>
+      <c r="B54" s="8"/>
       <c r="C54" s="3" t="s">
         <v>35</v>
       </c>
@@ -4960,10 +4957,10 @@
       <c r="Q54" s="2"/>
     </row>
     <row r="55" spans="1:17" ht="15" customHeight="1">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B55" s="6"/>
+      <c r="B55" s="8"/>
       <c r="C55" s="3" t="s">
         <v>35</v>
       </c>
@@ -5001,10 +4998,10 @@
       <c r="Q55" s="2"/>
     </row>
     <row r="56" spans="1:17" ht="15" customHeight="1">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="B56" s="6"/>
+      <c r="B56" s="8"/>
       <c r="C56" s="3" t="s">
         <v>35</v>
       </c>
@@ -5042,10 +5039,10 @@
       <c r="Q56" s="2"/>
     </row>
     <row r="57" spans="1:17" ht="15" customHeight="1">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="B57" s="6"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="3" t="s">
         <v>35</v>
       </c>
@@ -5083,10 +5080,10 @@
       <c r="Q57" s="2"/>
     </row>
     <row r="58" spans="1:17" ht="15" customHeight="1">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="B58" s="6"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="3" t="s">
         <v>35</v>
       </c>
@@ -5124,10 +5121,10 @@
       <c r="Q58" s="2"/>
     </row>
     <row r="59" spans="1:17" ht="15" customHeight="1">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="B59" s="6"/>
+      <c r="B59" s="8"/>
       <c r="C59" s="3" t="s">
         <v>35</v>
       </c>
@@ -5165,10 +5162,10 @@
       <c r="Q59" s="2"/>
     </row>
     <row r="60" spans="1:17" ht="15" customHeight="1">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="3" t="s">
         <v>35</v>
       </c>
@@ -5206,10 +5203,10 @@
       <c r="Q60" s="2"/>
     </row>
     <row r="61" spans="1:17" ht="15" customHeight="1">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="B61" s="6"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="3" t="s">
         <v>35</v>
       </c>
@@ -5247,10 +5244,10 @@
       <c r="Q61" s="2"/>
     </row>
     <row r="62" spans="1:17" ht="15" customHeight="1">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="8"/>
       <c r="C62" s="3" t="s">
         <v>35</v>
       </c>
@@ -5288,10 +5285,10 @@
       <c r="Q62" s="2"/>
     </row>
     <row r="63" spans="1:17" ht="15" customHeight="1">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="B63" s="6"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="3" t="s">
         <v>35</v>
       </c>
@@ -5329,10 +5326,10 @@
       <c r="Q63" s="2"/>
     </row>
     <row r="64" spans="1:17" ht="15" customHeight="1">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="8" t="s">
         <v>327</v>
       </c>
-      <c r="B64" s="6"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="3" t="s">
         <v>35</v>
       </c>
@@ -5370,10 +5367,10 @@
       <c r="Q64" s="2"/>
     </row>
     <row r="65" spans="1:17" ht="15" customHeight="1">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="B65" s="6"/>
+      <c r="B65" s="8"/>
       <c r="C65" s="3" t="s">
         <v>35</v>
       </c>
@@ -5411,10 +5408,10 @@
       <c r="Q65" s="2"/>
     </row>
     <row r="66" spans="1:17" ht="15" customHeight="1">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="B66" s="6"/>
+      <c r="B66" s="8"/>
       <c r="C66" s="3" t="s">
         <v>35</v>
       </c>
@@ -5452,10 +5449,10 @@
       <c r="Q66" s="2"/>
     </row>
     <row r="67" spans="1:17" ht="15" customHeight="1">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="B67" s="6"/>
+      <c r="B67" s="8"/>
       <c r="C67" s="3" t="s">
         <v>35</v>
       </c>
@@ -5493,10 +5490,10 @@
       <c r="Q67" s="2"/>
     </row>
     <row r="68" spans="1:17" ht="15" customHeight="1">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="B68" s="6"/>
+      <c r="B68" s="8"/>
       <c r="C68" s="3" t="s">
         <v>22</v>
       </c>
@@ -5534,10 +5531,10 @@
       <c r="Q68" s="2"/>
     </row>
     <row r="69" spans="1:17" ht="15" customHeight="1">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="B69" s="6"/>
+      <c r="B69" s="8"/>
       <c r="C69" s="3" t="s">
         <v>22</v>
       </c>
@@ -5575,10 +5572,10 @@
       <c r="Q69" s="2"/>
     </row>
     <row r="70" spans="1:17" ht="15" customHeight="1">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="B70" s="6"/>
+      <c r="B70" s="8"/>
       <c r="C70" s="3" t="s">
         <v>22</v>
       </c>
@@ -5616,10 +5613,10 @@
       <c r="Q70" s="2"/>
     </row>
     <row r="71" spans="1:17" ht="15" customHeight="1">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B71" s="6"/>
+      <c r="B71" s="8"/>
       <c r="C71" s="3" t="s">
         <v>22</v>
       </c>
@@ -5657,10 +5654,10 @@
       <c r="Q71" s="2"/>
     </row>
     <row r="72" spans="1:17" ht="15" customHeight="1">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B72" s="6"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="3" t="s">
         <v>22</v>
       </c>
@@ -5698,10 +5695,10 @@
       <c r="Q72" s="2"/>
     </row>
     <row r="73" spans="1:17" ht="15" customHeight="1">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="B73" s="6"/>
+      <c r="B73" s="8"/>
       <c r="C73" s="3" t="s">
         <v>22</v>
       </c>
@@ -5739,10 +5736,10 @@
       <c r="Q73" s="2"/>
     </row>
     <row r="74" spans="1:17" ht="15" customHeight="1">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="B74" s="6"/>
+      <c r="B74" s="8"/>
       <c r="C74" s="3" t="s">
         <v>22</v>
       </c>
@@ -5780,10 +5777,10 @@
       <c r="Q74" s="2"/>
     </row>
     <row r="75" spans="1:17" ht="15" customHeight="1">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="B75" s="6"/>
+      <c r="B75" s="8"/>
       <c r="C75" s="3" t="s">
         <v>22</v>
       </c>
@@ -5821,10 +5818,10 @@
       <c r="Q75" s="2"/>
     </row>
     <row r="76" spans="1:17" ht="15" customHeight="1">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="8" t="s">
         <v>385</v>
       </c>
-      <c r="B76" s="6"/>
+      <c r="B76" s="8"/>
       <c r="C76" s="3" t="s">
         <v>22</v>
       </c>
@@ -5862,10 +5859,10 @@
       <c r="Q76" s="2"/>
     </row>
     <row r="77" spans="1:17" ht="15" customHeight="1">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="8" t="s">
         <v>390</v>
       </c>
-      <c r="B77" s="6"/>
+      <c r="B77" s="8"/>
       <c r="C77" s="3" t="s">
         <v>22</v>
       </c>
@@ -5903,10 +5900,10 @@
       <c r="Q77" s="2"/>
     </row>
     <row r="78" spans="1:17" ht="15" customHeight="1">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="B78" s="6"/>
+      <c r="B78" s="8"/>
       <c r="C78" s="3" t="s">
         <v>22</v>
       </c>
@@ -5934,8 +5931,8 @@
       <c r="K78" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="L78" s="3" t="s">
-        <v>396</v>
+      <c r="L78" s="3">
+        <v>500</v>
       </c>
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
@@ -5944,10 +5941,10 @@
       <c r="Q78" s="2"/>
     </row>
     <row r="79" spans="1:17" ht="15" customHeight="1">
-      <c r="A79" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="B79" s="6"/>
+      <c r="A79" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B79" s="8"/>
       <c r="C79" s="3" t="s">
         <v>22</v>
       </c>
@@ -5976,7 +5973,7 @@
         <v>311</v>
       </c>
       <c r="L79" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
@@ -5985,10 +5982,10 @@
       <c r="Q79" s="2"/>
     </row>
     <row r="80" spans="1:17" ht="15" customHeight="1">
-      <c r="A80" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="B80" s="6"/>
+      <c r="A80" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B80" s="8"/>
       <c r="C80" s="3" t="s">
         <v>22</v>
       </c>
@@ -6005,19 +6002,19 @@
         <v>66</v>
       </c>
       <c r="H80" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="I80" s="3" t="s">
         <v>400</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>401</v>
       </c>
       <c r="J80" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K80" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="L80" s="3" t="s">
         <v>402</v>
-      </c>
-      <c r="L80" s="3" t="s">
-        <v>403</v>
       </c>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
@@ -6026,10 +6023,10 @@
       <c r="Q80" s="2"/>
     </row>
     <row r="81" spans="1:17" ht="15" customHeight="1">
-      <c r="A81" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="B81" s="6"/>
+      <c r="A81" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="B81" s="8"/>
       <c r="C81" s="3" t="s">
         <v>22</v>
       </c>
@@ -6046,16 +6043,16 @@
         <v>66</v>
       </c>
       <c r="H81" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="I81" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>406</v>
       </c>
       <c r="J81" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L81" s="3" t="s">
         <v>261</v>
@@ -6067,10 +6064,10 @@
       <c r="Q81" s="2"/>
     </row>
     <row r="82" spans="1:17" ht="15" customHeight="1">
-      <c r="A82" s="6" t="s">
-        <v>408</v>
-      </c>
-      <c r="B82" s="6"/>
+      <c r="A82" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="B82" s="8"/>
       <c r="C82" s="3" t="s">
         <v>22</v>
       </c>
@@ -6087,19 +6084,19 @@
         <v>66</v>
       </c>
       <c r="H82" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="I82" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>410</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K82" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="L82" s="3" t="s">
         <v>411</v>
-      </c>
-      <c r="L82" s="3" t="s">
-        <v>412</v>
       </c>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
@@ -6108,10 +6105,10 @@
       <c r="Q82" s="2"/>
     </row>
     <row r="83" spans="1:17" ht="15" customHeight="1">
-      <c r="A83" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="B83" s="6"/>
+      <c r="A83" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B83" s="8"/>
       <c r="C83" s="3" t="s">
         <v>22</v>
       </c>
@@ -6128,19 +6125,19 @@
         <v>66</v>
       </c>
       <c r="H83" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="I83" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>415</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K83" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="L83" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="L83" s="3" t="s">
-        <v>417</v>
       </c>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
@@ -6149,10 +6146,10 @@
       <c r="Q83" s="2"/>
     </row>
     <row r="84" spans="1:17" ht="15" customHeight="1">
-      <c r="A84" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="B84" s="6"/>
+      <c r="A84" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B84" s="8"/>
       <c r="C84" s="3" t="s">
         <v>22</v>
       </c>
@@ -6172,13 +6169,13 @@
         <v>81</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="L84" s="3" t="s">
         <v>261</v>
@@ -6190,10 +6187,10 @@
       <c r="Q84" s="2"/>
     </row>
     <row r="85" spans="1:17" ht="15" customHeight="1">
-      <c r="A85" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="B85" s="6"/>
+      <c r="A85" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="B85" s="8"/>
       <c r="C85" s="3" t="s">
         <v>22</v>
       </c>
@@ -6210,19 +6207,19 @@
         <v>66</v>
       </c>
       <c r="H85" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>422</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>423</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K85" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="L85" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="L85" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
@@ -6231,10 +6228,10 @@
       <c r="Q85" s="2"/>
     </row>
     <row r="86" spans="1:17" ht="15" customHeight="1">
-      <c r="A86" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="B86" s="6"/>
+      <c r="A86" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="B86" s="8"/>
       <c r="C86" s="3" t="s">
         <v>22</v>
       </c>
@@ -6251,19 +6248,19 @@
         <v>66</v>
       </c>
       <c r="H86" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="I86" s="3" t="s">
         <v>427</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>428</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K86" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="L86" s="3" t="s">
         <v>429</v>
-      </c>
-      <c r="L86" s="3" t="s">
-        <v>430</v>
       </c>
       <c r="M86" s="3"/>
       <c r="N86" s="3"/>
@@ -6272,10 +6269,10 @@
       <c r="Q86" s="2"/>
     </row>
     <row r="87" spans="1:17" ht="15" customHeight="1">
-      <c r="A87" s="6" t="s">
-        <v>431</v>
-      </c>
-      <c r="B87" s="6"/>
+      <c r="A87" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="B87" s="8"/>
       <c r="C87" s="3" t="s">
         <v>22</v>
       </c>
@@ -6292,19 +6289,19 @@
         <v>66</v>
       </c>
       <c r="H87" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="I87" s="3" t="s">
         <v>432</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>433</v>
       </c>
       <c r="J87" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K87" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="L87" s="3" t="s">
         <v>434</v>
-      </c>
-      <c r="L87" s="3" t="s">
-        <v>435</v>
       </c>
       <c r="M87" s="3"/>
       <c r="N87" s="3"/>
@@ -6313,10 +6310,10 @@
       <c r="Q87" s="2"/>
     </row>
     <row r="88" spans="1:17" ht="15" customHeight="1">
-      <c r="A88" s="6" t="s">
-        <v>436</v>
-      </c>
-      <c r="B88" s="6"/>
+      <c r="A88" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="B88" s="8"/>
       <c r="C88" s="3" t="s">
         <v>64</v>
       </c>
@@ -6333,19 +6330,19 @@
         <v>66</v>
       </c>
       <c r="H88" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="I88" s="3" t="s">
         <v>437</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>438</v>
       </c>
       <c r="J88" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K88" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="L88" s="3" t="s">
         <v>439</v>
-      </c>
-      <c r="L88" s="3" t="s">
-        <v>440</v>
       </c>
       <c r="M88" s="3"/>
       <c r="N88" s="3"/>
@@ -6354,10 +6351,10 @@
       <c r="Q88" s="2"/>
     </row>
     <row r="89" spans="1:17" ht="15" customHeight="1">
-      <c r="A89" s="6" t="s">
-        <v>441</v>
-      </c>
-      <c r="B89" s="6"/>
+      <c r="A89" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="B89" s="8"/>
       <c r="C89" s="3" t="s">
         <v>64</v>
       </c>
@@ -6374,19 +6371,19 @@
         <v>66</v>
       </c>
       <c r="H89" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="I89" s="3" t="s">
         <v>442</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>443</v>
       </c>
       <c r="J89" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K89" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="L89" s="3" t="s">
         <v>444</v>
-      </c>
-      <c r="L89" s="3" t="s">
-        <v>445</v>
       </c>
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
@@ -6395,10 +6392,10 @@
       <c r="Q89" s="2"/>
     </row>
     <row r="90" spans="1:17" ht="15" customHeight="1">
-      <c r="A90" s="6">
+      <c r="A90" s="8">
         <v>763190794566</v>
       </c>
-      <c r="B90" s="6"/>
+      <c r="B90" s="8"/>
       <c r="C90" s="3" t="s">
         <v>64</v>
       </c>
@@ -6415,19 +6412,19 @@
         <v>66</v>
       </c>
       <c r="H90" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="I90" s="3" t="s">
         <v>446</v>
-      </c>
-      <c r="I90" s="3" t="s">
-        <v>447</v>
       </c>
       <c r="J90" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K90" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="L90" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="M90" s="3"/>
       <c r="N90" s="3"/>
@@ -6436,10 +6433,10 @@
       <c r="Q90" s="2"/>
     </row>
     <row r="91" spans="1:17" ht="15" customHeight="1">
-      <c r="A91" s="6" t="s">
-        <v>449</v>
-      </c>
-      <c r="B91" s="6"/>
+      <c r="A91" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="B91" s="8"/>
       <c r="C91" s="3" t="s">
         <v>64</v>
       </c>
@@ -6456,19 +6453,19 @@
         <v>66</v>
       </c>
       <c r="H91" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="I91" s="3" t="s">
         <v>450</v>
-      </c>
-      <c r="I91" s="3" t="s">
-        <v>451</v>
       </c>
       <c r="J91" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K91" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="L91" s="3" t="s">
         <v>452</v>
-      </c>
-      <c r="L91" s="3" t="s">
-        <v>453</v>
       </c>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
@@ -6477,10 +6474,10 @@
       <c r="Q91" s="2"/>
     </row>
     <row r="92" spans="1:17" ht="15" customHeight="1">
-      <c r="A92" s="6" t="s">
-        <v>454</v>
-      </c>
-      <c r="B92" s="6"/>
+      <c r="A92" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B92" s="8"/>
       <c r="C92" s="3" t="s">
         <v>64</v>
       </c>
@@ -6497,16 +6494,16 @@
         <v>66</v>
       </c>
       <c r="H92" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="I92" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="I92" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="J92" s="3" t="s">
         <v>193</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="L92" s="3" t="s">
         <v>261</v>
@@ -6518,10 +6515,10 @@
       <c r="Q92" s="2"/>
     </row>
     <row r="93" spans="1:17" ht="15" customHeight="1">
-      <c r="A93" s="6" t="s">
-        <v>458</v>
-      </c>
-      <c r="B93" s="6"/>
+      <c r="A93" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B93" s="8"/>
       <c r="C93" s="3" t="s">
         <v>58</v>
       </c>
@@ -6538,19 +6535,19 @@
         <v>66</v>
       </c>
       <c r="H93" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="I93" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="I93" s="3" t="s">
+      <c r="J93" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="J93" s="3" t="s">
+      <c r="K93" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="K93" s="3" t="s">
+      <c r="L93" s="3" t="s">
         <v>462</v>
-      </c>
-      <c r="L93" s="3" t="s">
-        <v>463</v>
       </c>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
@@ -6559,10 +6556,10 @@
       <c r="Q93" s="2"/>
     </row>
     <row r="94" spans="1:17" ht="15" customHeight="1">
-      <c r="A94" s="6" t="s">
-        <v>464</v>
-      </c>
-      <c r="B94" s="6"/>
+      <c r="A94" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B94" s="8"/>
       <c r="C94" s="3" t="s">
         <v>58</v>
       </c>
@@ -6579,19 +6576,19 @@
         <v>66</v>
       </c>
       <c r="H94" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="I94" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="I94" s="3" t="s">
+      <c r="J94" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K94" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="J94" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K94" s="3" t="s">
+      <c r="L94" s="3" t="s">
         <v>467</v>
-      </c>
-      <c r="L94" s="3" t="s">
-        <v>468</v>
       </c>
       <c r="M94" s="3"/>
       <c r="N94" s="3"/>
@@ -6600,10 +6597,10 @@
       <c r="Q94" s="2"/>
     </row>
     <row r="95" spans="1:17" ht="15" customHeight="1">
-      <c r="A95" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="B95" s="6"/>
+      <c r="A95" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="B95" s="8"/>
       <c r="C95" s="3" t="s">
         <v>58</v>
       </c>
@@ -6614,25 +6611,25 @@
         <v>37</v>
       </c>
       <c r="F95" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H95" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="G95" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H95" s="3" t="s">
+      <c r="I95" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="I95" s="3" t="s">
+      <c r="J95" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K95" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="J95" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K95" s="3" t="s">
+      <c r="L95" s="3" t="s">
         <v>473</v>
-      </c>
-      <c r="L95" s="3" t="s">
-        <v>474</v>
       </c>
       <c r="M95" s="3"/>
       <c r="N95" s="3"/>
@@ -6641,10 +6638,10 @@
       <c r="Q95" s="2"/>
     </row>
     <row r="96" spans="1:17" ht="15" customHeight="1">
-      <c r="A96" s="6" t="s">
-        <v>475</v>
-      </c>
-      <c r="B96" s="6"/>
+      <c r="A96" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="B96" s="8"/>
       <c r="C96" s="3" t="s">
         <v>130</v>
       </c>
@@ -6661,19 +6658,19 @@
         <v>66</v>
       </c>
       <c r="H96" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="I96" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="I96" s="3" t="s">
+      <c r="J96" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K96" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="J96" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K96" s="3" t="s">
+      <c r="L96" s="3" t="s">
         <v>478</v>
-      </c>
-      <c r="L96" s="3" t="s">
-        <v>479</v>
       </c>
       <c r="M96" s="3"/>
       <c r="N96" s="3"/>
@@ -6682,10 +6679,10 @@
       <c r="Q96" s="2"/>
     </row>
     <row r="97" spans="1:17" ht="15" customHeight="1">
-      <c r="A97" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="B97" s="6"/>
+      <c r="A97" s="8" t="s">
+        <v>479</v>
+      </c>
+      <c r="B97" s="8"/>
       <c r="C97" s="3" t="s">
         <v>268</v>
       </c>
@@ -6702,19 +6699,19 @@
         <v>66</v>
       </c>
       <c r="H97" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="I97" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="I97" s="3" t="s">
+      <c r="J97" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K97" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="J97" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K97" s="3" t="s">
+      <c r="L97" s="3" t="s">
         <v>483</v>
-      </c>
-      <c r="L97" s="3" t="s">
-        <v>484</v>
       </c>
       <c r="M97" s="3"/>
       <c r="N97" s="3"/>
@@ -6723,10 +6720,10 @@
       <c r="Q97" s="2"/>
     </row>
     <row r="98" spans="1:17" ht="15" customHeight="1">
-      <c r="A98" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="B98" s="6"/>
+      <c r="A98" s="8" t="s">
+        <v>484</v>
+      </c>
+      <c r="B98" s="8"/>
       <c r="C98" s="3" t="s">
         <v>35</v>
       </c>
@@ -6743,19 +6740,19 @@
         <v>66</v>
       </c>
       <c r="H98" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="I98" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="I98" s="3" t="s">
+      <c r="J98" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K98" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="J98" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K98" s="3" t="s">
+      <c r="L98" s="3" t="s">
         <v>488</v>
-      </c>
-      <c r="L98" s="3" t="s">
-        <v>489</v>
       </c>
       <c r="M98" s="3"/>
       <c r="N98" s="3"/>
@@ -6764,10 +6761,10 @@
       <c r="Q98" s="2"/>
     </row>
     <row r="99" spans="1:17" ht="15" customHeight="1">
-      <c r="A99" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="B99" s="6"/>
+      <c r="A99" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="B99" s="8"/>
       <c r="C99" s="3" t="s">
         <v>35</v>
       </c>
@@ -6784,19 +6781,19 @@
         <v>66</v>
       </c>
       <c r="H99" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="I99" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="I99" s="3" t="s">
+      <c r="J99" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K99" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="J99" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K99" s="3" t="s">
+      <c r="L99" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="L99" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="M99" s="3"/>
       <c r="N99" s="3"/>
@@ -6805,10 +6802,10 @@
       <c r="Q99" s="2"/>
     </row>
     <row r="100" spans="1:17" ht="15" customHeight="1">
-      <c r="A100" s="6" t="s">
-        <v>495</v>
-      </c>
-      <c r="B100" s="6"/>
+      <c r="A100" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="B100" s="8"/>
       <c r="C100" s="3" t="s">
         <v>35</v>
       </c>
@@ -6825,19 +6822,19 @@
         <v>66</v>
       </c>
       <c r="H100" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="I100" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="I100" s="3" t="s">
+      <c r="J100" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K100" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="J100" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K100" s="3" t="s">
+      <c r="L100" s="3" t="s">
         <v>498</v>
-      </c>
-      <c r="L100" s="3" t="s">
-        <v>499</v>
       </c>
       <c r="M100" s="3"/>
       <c r="N100" s="3"/>
@@ -6846,10 +6843,10 @@
       <c r="Q100" s="2"/>
     </row>
     <row r="101" spans="1:17" ht="15" customHeight="1">
-      <c r="A101" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="B101" s="6"/>
+      <c r="A101" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B101" s="8"/>
       <c r="C101" s="3" t="s">
         <v>35</v>
       </c>
@@ -6866,19 +6863,19 @@
         <v>66</v>
       </c>
       <c r="H101" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="I101" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="I101" s="3" t="s">
+      <c r="J101" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K101" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="J101" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K101" s="3" t="s">
+      <c r="L101" s="3" t="s">
         <v>503</v>
-      </c>
-      <c r="L101" s="3" t="s">
-        <v>504</v>
       </c>
       <c r="M101" s="3"/>
       <c r="N101" s="3"/>
@@ -6887,10 +6884,10 @@
       <c r="Q101" s="2"/>
     </row>
     <row r="102" spans="1:17" ht="15" customHeight="1">
-      <c r="A102" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="B102" s="6"/>
+      <c r="A102" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="B102" s="8"/>
       <c r="C102" s="3" t="s">
         <v>35</v>
       </c>
@@ -6907,19 +6904,19 @@
         <v>66</v>
       </c>
       <c r="H102" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="I102" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="I102" s="3" t="s">
+      <c r="J102" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K102" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="J102" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K102" s="3" t="s">
+      <c r="L102" s="3" t="s">
         <v>508</v>
-      </c>
-      <c r="L102" s="3" t="s">
-        <v>509</v>
       </c>
       <c r="M102" s="3"/>
       <c r="N102" s="3"/>
@@ -6928,10 +6925,10 @@
       <c r="Q102" s="2"/>
     </row>
     <row r="103" spans="1:17" ht="15" customHeight="1">
-      <c r="A103" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="B103" s="6"/>
+      <c r="A103" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="B103" s="8"/>
       <c r="C103" s="3" t="s">
         <v>35</v>
       </c>
@@ -6948,19 +6945,19 @@
         <v>66</v>
       </c>
       <c r="H103" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="I103" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="I103" s="3" t="s">
+      <c r="J103" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K103" s="3" t="s">
         <v>512</v>
       </c>
-      <c r="J103" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K103" s="3" t="s">
+      <c r="L103" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="L103" s="3" t="s">
-        <v>514</v>
       </c>
       <c r="M103" s="3"/>
       <c r="N103" s="3"/>
@@ -6969,10 +6966,10 @@
       <c r="Q103" s="2"/>
     </row>
     <row r="104" spans="1:17" ht="15" customHeight="1">
-      <c r="A104" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="B104" s="6"/>
+      <c r="A104" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="B104" s="8"/>
       <c r="C104" s="3" t="s">
         <v>22</v>
       </c>
@@ -6989,19 +6986,19 @@
         <v>66</v>
       </c>
       <c r="H104" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="I104" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="I104" s="3" t="s">
+      <c r="J104" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K104" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="J104" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K104" s="3" t="s">
+      <c r="L104" s="3" t="s">
         <v>518</v>
-      </c>
-      <c r="L104" s="3" t="s">
-        <v>519</v>
       </c>
       <c r="M104" s="3"/>
       <c r="N104" s="3"/>
@@ -7010,10 +7007,10 @@
       <c r="Q104" s="2"/>
     </row>
     <row r="105" spans="1:17" ht="15" customHeight="1">
-      <c r="A105" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="B105" s="6"/>
+      <c r="A105" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="B105" s="8"/>
       <c r="C105" s="3" t="s">
         <v>22</v>
       </c>
@@ -7030,19 +7027,19 @@
         <v>66</v>
       </c>
       <c r="H105" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="I105" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="I105" s="3" t="s">
+      <c r="J105" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K105" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="J105" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K105" s="3" t="s">
+      <c r="L105" s="3" t="s">
         <v>523</v>
-      </c>
-      <c r="L105" s="3" t="s">
-        <v>524</v>
       </c>
       <c r="M105" s="3"/>
       <c r="N105" s="3"/>
@@ -7051,10 +7048,10 @@
       <c r="Q105" s="2"/>
     </row>
     <row r="106" spans="1:17" ht="15" customHeight="1">
-      <c r="A106" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="B106" s="6"/>
+      <c r="A106" s="8" t="s">
+        <v>524</v>
+      </c>
+      <c r="B106" s="8"/>
       <c r="C106" s="3" t="s">
         <v>22</v>
       </c>
@@ -7071,19 +7068,19 @@
         <v>66</v>
       </c>
       <c r="H106" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="I106" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="I106" s="3" t="s">
+      <c r="J106" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K106" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="J106" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K106" s="3" t="s">
+      <c r="L106" s="3" t="s">
         <v>528</v>
-      </c>
-      <c r="L106" s="3" t="s">
-        <v>529</v>
       </c>
       <c r="M106" s="3"/>
       <c r="N106" s="3"/>
@@ -7092,10 +7089,10 @@
       <c r="Q106" s="2"/>
     </row>
     <row r="107" spans="1:17" ht="15" customHeight="1">
-      <c r="A107" s="6" t="s">
-        <v>530</v>
-      </c>
-      <c r="B107" s="6"/>
+      <c r="A107" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="B107" s="8"/>
       <c r="C107" s="3" t="s">
         <v>22</v>
       </c>
@@ -7112,19 +7109,19 @@
         <v>66</v>
       </c>
       <c r="H107" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="I107" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="I107" s="3" t="s">
+      <c r="J107" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K107" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="J107" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K107" s="3" t="s">
+      <c r="L107" s="3" t="s">
         <v>533</v>
-      </c>
-      <c r="L107" s="3" t="s">
-        <v>534</v>
       </c>
       <c r="M107" s="3"/>
       <c r="N107" s="3"/>
@@ -7133,10 +7130,10 @@
       <c r="Q107" s="2"/>
     </row>
     <row r="108" spans="1:17" ht="15" customHeight="1">
-      <c r="A108" s="6" t="s">
-        <v>535</v>
-      </c>
-      <c r="B108" s="6"/>
+      <c r="A108" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="B108" s="8"/>
       <c r="C108" s="3" t="s">
         <v>22</v>
       </c>
@@ -7153,19 +7150,19 @@
         <v>66</v>
       </c>
       <c r="H108" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="I108" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="I108" s="3" t="s">
+      <c r="J108" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K108" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="J108" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K108" s="3" t="s">
+      <c r="L108" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="L108" s="3" t="s">
-        <v>539</v>
       </c>
       <c r="M108" s="3"/>
       <c r="N108" s="3"/>
@@ -7174,10 +7171,10 @@
       <c r="Q108" s="2"/>
     </row>
     <row r="109" spans="1:17" ht="15" customHeight="1">
-      <c r="A109" s="6" t="s">
-        <v>540</v>
-      </c>
-      <c r="B109" s="6"/>
+      <c r="A109" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="B109" s="8"/>
       <c r="C109" s="3" t="s">
         <v>22</v>
       </c>
@@ -7194,19 +7191,19 @@
         <v>66</v>
       </c>
       <c r="H109" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="I109" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="I109" s="3" t="s">
+      <c r="J109" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K109" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="J109" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K109" s="3" t="s">
+      <c r="L109" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="L109" s="3" t="s">
-        <v>544</v>
       </c>
       <c r="M109" s="3"/>
       <c r="N109" s="3"/>
@@ -7215,10 +7212,10 @@
       <c r="Q109" s="2"/>
     </row>
     <row r="110" spans="1:17" ht="15" customHeight="1">
-      <c r="A110" s="6" t="s">
-        <v>545</v>
-      </c>
-      <c r="B110" s="6"/>
+      <c r="A110" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="B110" s="8"/>
       <c r="C110" s="3" t="s">
         <v>22</v>
       </c>
@@ -7235,19 +7232,19 @@
         <v>66</v>
       </c>
       <c r="H110" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="I110" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="I110" s="3" t="s">
+      <c r="J110" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K110" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="J110" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K110" s="3" t="s">
+      <c r="L110" s="3" t="s">
         <v>548</v>
-      </c>
-      <c r="L110" s="3" t="s">
-        <v>549</v>
       </c>
       <c r="M110" s="3"/>
       <c r="N110" s="3"/>
@@ -7256,10 +7253,10 @@
       <c r="Q110" s="2"/>
     </row>
     <row r="111" spans="1:17" ht="15" customHeight="1">
-      <c r="A111" s="6" t="s">
-        <v>550</v>
-      </c>
-      <c r="B111" s="6"/>
+      <c r="A111" s="8" t="s">
+        <v>549</v>
+      </c>
+      <c r="B111" s="8"/>
       <c r="C111" s="3" t="s">
         <v>22</v>
       </c>
@@ -7276,19 +7273,19 @@
         <v>66</v>
       </c>
       <c r="H111" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="I111" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="I111" s="3" t="s">
+      <c r="J111" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K111" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="J111" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K111" s="3" t="s">
+      <c r="L111" s="3" t="s">
         <v>553</v>
-      </c>
-      <c r="L111" s="3" t="s">
-        <v>554</v>
       </c>
       <c r="M111" s="3"/>
       <c r="N111" s="3"/>
@@ -7297,10 +7294,10 @@
       <c r="Q111" s="2"/>
     </row>
     <row r="112" spans="1:17" ht="15" customHeight="1">
-      <c r="A112" s="6" t="s">
-        <v>555</v>
-      </c>
-      <c r="B112" s="6"/>
+      <c r="A112" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="B112" s="8"/>
       <c r="C112" s="3" t="s">
         <v>22</v>
       </c>
@@ -7317,19 +7314,19 @@
         <v>66</v>
       </c>
       <c r="H112" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="I112" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="I112" s="3" t="s">
+      <c r="J112" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K112" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="J112" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K112" s="3" t="s">
+      <c r="L112" s="3" t="s">
         <v>558</v>
-      </c>
-      <c r="L112" s="3" t="s">
-        <v>559</v>
       </c>
       <c r="M112" s="3"/>
       <c r="N112" s="3"/>
@@ -7338,10 +7335,10 @@
       <c r="Q112" s="2"/>
     </row>
     <row r="113" spans="1:17" ht="15" customHeight="1">
-      <c r="A113" s="6" t="s">
-        <v>560</v>
-      </c>
-      <c r="B113" s="6"/>
+      <c r="A113" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="B113" s="8"/>
       <c r="C113" s="3" t="s">
         <v>64</v>
       </c>
@@ -7358,19 +7355,19 @@
         <v>66</v>
       </c>
       <c r="H113" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="I113" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="I113" s="3" t="s">
+      <c r="J113" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K113" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="J113" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K113" s="3" t="s">
+      <c r="L113" s="3" t="s">
         <v>563</v>
-      </c>
-      <c r="L113" s="3" t="s">
-        <v>564</v>
       </c>
       <c r="M113" s="3"/>
       <c r="N113" s="3"/>
@@ -7379,10 +7376,10 @@
       <c r="Q113" s="2"/>
     </row>
     <row r="114" spans="1:17" ht="15" customHeight="1">
-      <c r="A114" s="6" t="s">
-        <v>565</v>
-      </c>
-      <c r="B114" s="6"/>
+      <c r="A114" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="B114" s="8"/>
       <c r="C114" s="3" t="s">
         <v>64</v>
       </c>
@@ -7399,19 +7396,19 @@
         <v>66</v>
       </c>
       <c r="H114" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="I114" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="I114" s="3" t="s">
+      <c r="J114" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K114" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="J114" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K114" s="3" t="s">
-        <v>538</v>
-      </c>
       <c r="L114" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M114" s="3"/>
       <c r="N114" s="3"/>
@@ -7420,10 +7417,10 @@
       <c r="Q114" s="2"/>
     </row>
     <row r="115" spans="1:17" ht="15" customHeight="1">
-      <c r="A115" s="6" t="s">
-        <v>567</v>
-      </c>
-      <c r="B115" s="6"/>
+      <c r="A115" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="B115" s="8"/>
       <c r="C115" s="3" t="s">
         <v>64</v>
       </c>
@@ -7440,19 +7437,19 @@
         <v>66</v>
       </c>
       <c r="H115" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="I115" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="I115" s="3" t="s">
+      <c r="J115" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="K115" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="J115" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="K115" s="3" t="s">
+      <c r="L115" s="3" t="s">
         <v>570</v>
-      </c>
-      <c r="L115" s="3" t="s">
-        <v>571</v>
       </c>
       <c r="M115" s="3"/>
       <c r="N115" s="3"/>
@@ -7461,10 +7458,10 @@
       <c r="Q115" s="2"/>
     </row>
     <row r="116" spans="1:17" ht="15" customHeight="1">
-      <c r="A116" s="6" t="s">
-        <v>572</v>
-      </c>
-      <c r="B116" s="6"/>
+      <c r="A116" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="B116" s="8"/>
       <c r="C116" s="3" t="s">
         <v>22</v>
       </c>
@@ -7481,19 +7478,19 @@
         <v>66</v>
       </c>
       <c r="H116" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="I116" s="3" t="s">
         <v>573</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>574</v>
       </c>
       <c r="J116" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K116" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="L116" s="3" t="s">
         <v>575</v>
-      </c>
-      <c r="L116" s="3" t="s">
-        <v>576</v>
       </c>
       <c r="M116" s="3"/>
       <c r="N116" s="3"/>
@@ -7502,10 +7499,10 @@
       <c r="Q116" s="2"/>
     </row>
     <row r="117" spans="1:17" ht="15" customHeight="1">
-      <c r="A117" s="6" t="s">
-        <v>577</v>
-      </c>
-      <c r="B117" s="6"/>
+      <c r="A117" s="8" t="s">
+        <v>576</v>
+      </c>
+      <c r="B117" s="8"/>
       <c r="C117" s="3" t="s">
         <v>35</v>
       </c>
@@ -7522,19 +7519,19 @@
         <v>66</v>
       </c>
       <c r="H117" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="I117" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="I117" s="3" t="s">
+      <c r="J117" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="J117" s="3" t="s">
+      <c r="K117" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="K117" s="3" t="s">
+      <c r="L117" s="3" t="s">
         <v>581</v>
-      </c>
-      <c r="L117" s="3" t="s">
-        <v>582</v>
       </c>
       <c r="M117" s="3"/>
       <c r="N117" s="3"/>
@@ -7543,10 +7540,10 @@
       <c r="Q117" s="2"/>
     </row>
     <row r="118" spans="1:17" ht="15" customHeight="1">
-      <c r="A118" s="6" t="s">
-        <v>583</v>
-      </c>
-      <c r="B118" s="6"/>
+      <c r="A118" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="B118" s="8"/>
       <c r="C118" s="3" t="s">
         <v>130</v>
       </c>
@@ -7563,16 +7560,16 @@
         <v>66</v>
       </c>
       <c r="H118" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="I118" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="I118" s="3" t="s">
+      <c r="J118" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="J118" s="3" t="s">
+      <c r="K118" s="3" t="s">
         <v>586</v>
-      </c>
-      <c r="K118" s="3" t="s">
-        <v>587</v>
       </c>
       <c r="L118" s="3" t="s">
         <v>261</v>
@@ -7584,10 +7581,10 @@
       <c r="Q118" s="2"/>
     </row>
     <row r="119" spans="1:17" ht="15" customHeight="1">
-      <c r="A119" s="6" t="s">
-        <v>588</v>
-      </c>
-      <c r="B119" s="6"/>
+      <c r="A119" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="B119" s="8"/>
       <c r="C119" s="3" t="s">
         <v>35</v>
       </c>
@@ -7604,19 +7601,19 @@
         <v>66</v>
       </c>
       <c r="H119" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="I119" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="I119" s="3" t="s">
+      <c r="J119" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="K119" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="J119" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="K119" s="3" t="s">
+      <c r="L119" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="L119" s="3" t="s">
-        <v>592</v>
       </c>
       <c r="M119" s="3"/>
       <c r="N119" s="3"/>
@@ -7625,10 +7622,10 @@
       <c r="Q119" s="2"/>
     </row>
     <row r="120" spans="1:17" ht="15" customHeight="1">
-      <c r="A120" s="6" t="s">
-        <v>593</v>
-      </c>
-      <c r="B120" s="6"/>
+      <c r="A120" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="B120" s="8"/>
       <c r="C120" s="3" t="s">
         <v>22</v>
       </c>
@@ -7645,19 +7642,19 @@
         <v>66</v>
       </c>
       <c r="H120" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="I120" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="I120" s="3" t="s">
+      <c r="J120" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="K120" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="J120" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="K120" s="3" t="s">
+      <c r="L120" s="3" t="s">
         <v>596</v>
-      </c>
-      <c r="L120" s="3" t="s">
-        <v>597</v>
       </c>
       <c r="M120" s="3"/>
       <c r="N120" s="3"/>
@@ -7666,10 +7663,10 @@
       <c r="Q120" s="2"/>
     </row>
     <row r="121" spans="1:17" ht="15" customHeight="1">
-      <c r="A121" s="6" t="s">
-        <v>598</v>
-      </c>
-      <c r="B121" s="6"/>
+      <c r="A121" s="8" t="s">
+        <v>597</v>
+      </c>
+      <c r="B121" s="8"/>
       <c r="C121" s="3" t="s">
         <v>22</v>
       </c>
@@ -7686,19 +7683,19 @@
         <v>66</v>
       </c>
       <c r="H121" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="I121" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="I121" s="3" t="s">
+      <c r="J121" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="K121" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="J121" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="K121" s="3" t="s">
+      <c r="L121" s="3" t="s">
         <v>601</v>
-      </c>
-      <c r="L121" s="3" t="s">
-        <v>602</v>
       </c>
       <c r="M121" s="3"/>
       <c r="N121" s="3"/>
@@ -7707,10 +7704,10 @@
       <c r="Q121" s="2"/>
     </row>
     <row r="122" spans="1:17" ht="15" customHeight="1">
-      <c r="A122" s="6" t="s">
-        <v>603</v>
-      </c>
-      <c r="B122" s="6"/>
+      <c r="A122" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="B122" s="8"/>
       <c r="C122" s="3" t="s">
         <v>22</v>
       </c>
@@ -7727,19 +7724,19 @@
         <v>66</v>
       </c>
       <c r="H122" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="I122" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="I122" s="3" t="s">
+      <c r="J122" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="K122" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="J122" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="K122" s="3" t="s">
+      <c r="L122" s="3" t="s">
         <v>606</v>
-      </c>
-      <c r="L122" s="3" t="s">
-        <v>607</v>
       </c>
       <c r="M122" s="3"/>
       <c r="N122" s="3"/>
@@ -7748,10 +7745,10 @@
       <c r="Q122" s="2"/>
     </row>
     <row r="123" spans="1:17" ht="15" customHeight="1">
-      <c r="A123" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="B123" s="6"/>
+      <c r="A123" s="8" t="s">
+        <v>607</v>
+      </c>
+      <c r="B123" s="8"/>
       <c r="C123" s="3" t="s">
         <v>44</v>
       </c>
@@ -7768,19 +7765,19 @@
         <v>66</v>
       </c>
       <c r="H123" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="I123" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="I123" s="3" t="s">
+      <c r="J123" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="J123" s="3" t="s">
+      <c r="K123" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="K123" s="3" t="s">
+      <c r="L123" s="3" t="s">
         <v>612</v>
-      </c>
-      <c r="L123" s="3" t="s">
-        <v>613</v>
       </c>
       <c r="M123" s="3"/>
       <c r="N123" s="3"/>
@@ -7789,10 +7786,10 @@
       <c r="Q123" s="2"/>
     </row>
     <row r="124" spans="1:17" ht="15" customHeight="1">
-      <c r="A124" s="6" t="s">
-        <v>614</v>
-      </c>
-      <c r="B124" s="6"/>
+      <c r="A124" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="B124" s="8"/>
       <c r="C124" s="3" t="s">
         <v>44</v>
       </c>
@@ -7809,19 +7806,19 @@
         <v>66</v>
       </c>
       <c r="H124" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="I124" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="I124" s="3" t="s">
+      <c r="J124" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="K124" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="J124" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="K124" s="3" t="s">
+      <c r="L124" s="3" t="s">
         <v>617</v>
-      </c>
-      <c r="L124" s="3" t="s">
-        <v>618</v>
       </c>
       <c r="M124" s="3"/>
       <c r="N124" s="3"/>
@@ -7830,10 +7827,10 @@
       <c r="Q124" s="2"/>
     </row>
     <row r="125" spans="1:17" ht="15" customHeight="1">
-      <c r="A125" s="6" t="s">
-        <v>619</v>
-      </c>
-      <c r="B125" s="6"/>
+      <c r="A125" s="8" t="s">
+        <v>618</v>
+      </c>
+      <c r="B125" s="8"/>
       <c r="C125" s="3" t="s">
         <v>22</v>
       </c>
@@ -7850,19 +7847,19 @@
         <v>66</v>
       </c>
       <c r="H125" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="I125" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="I125" s="3" t="s">
+      <c r="J125" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="K125" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="J125" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="K125" s="3" t="s">
+      <c r="L125" s="3" t="s">
         <v>622</v>
-      </c>
-      <c r="L125" s="3" t="s">
-        <v>623</v>
       </c>
       <c r="M125" s="3"/>
       <c r="N125" s="3"/>
@@ -7871,10 +7868,10 @@
       <c r="Q125" s="2"/>
     </row>
     <row r="126" spans="1:17" ht="15" customHeight="1">
-      <c r="A126" s="6" t="s">
-        <v>624</v>
-      </c>
-      <c r="B126" s="6"/>
+      <c r="A126" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="B126" s="8"/>
       <c r="C126" s="3" t="s">
         <v>64</v>
       </c>
@@ -7891,19 +7888,19 @@
         <v>66</v>
       </c>
       <c r="H126" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="I126" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="I126" s="3" t="s">
+      <c r="J126" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="K126" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="J126" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="K126" s="3" t="s">
+      <c r="L126" s="3" t="s">
         <v>627</v>
-      </c>
-      <c r="L126" s="3" t="s">
-        <v>628</v>
       </c>
       <c r="M126" s="3"/>
       <c r="N126" s="3"/>
@@ -7912,10 +7909,10 @@
       <c r="Q126" s="2"/>
     </row>
     <row r="127" spans="1:17" ht="15" customHeight="1">
-      <c r="A127" s="6" t="s">
-        <v>629</v>
-      </c>
-      <c r="B127" s="6"/>
+      <c r="A127" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="B127" s="8"/>
       <c r="C127" s="3" t="s">
         <v>64</v>
       </c>
@@ -7932,19 +7929,19 @@
         <v>66</v>
       </c>
       <c r="H127" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="I127" s="3" t="s">
         <v>630</v>
-      </c>
-      <c r="I127" s="3" t="s">
-        <v>631</v>
       </c>
       <c r="J127" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K127" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="L127" s="3" t="s">
         <v>632</v>
-      </c>
-      <c r="L127" s="3" t="s">
-        <v>633</v>
       </c>
       <c r="M127" s="3"/>
       <c r="N127" s="3"/>
@@ -7953,10 +7950,10 @@
       <c r="Q127" s="2"/>
     </row>
     <row r="128" spans="1:17" ht="15" customHeight="1">
-      <c r="A128" s="6" t="s">
-        <v>634</v>
-      </c>
-      <c r="B128" s="6"/>
+      <c r="A128" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="B128" s="8"/>
       <c r="C128" s="3" t="s">
         <v>35</v>
       </c>
@@ -7973,19 +7970,19 @@
         <v>66</v>
       </c>
       <c r="H128" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="I128" s="3" t="s">
         <v>635</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>636</v>
       </c>
       <c r="J128" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K128" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="L128" s="3" t="s">
         <v>637</v>
-      </c>
-      <c r="L128" s="3" t="s">
-        <v>638</v>
       </c>
       <c r="M128" s="3"/>
       <c r="N128" s="3"/>
@@ -7994,10 +7991,10 @@
       <c r="Q128" s="2"/>
     </row>
     <row r="129" spans="1:17" ht="15" customHeight="1">
-      <c r="A129" s="6" t="s">
-        <v>639</v>
-      </c>
-      <c r="B129" s="6"/>
+      <c r="A129" s="8" t="s">
+        <v>638</v>
+      </c>
+      <c r="B129" s="8"/>
       <c r="C129" s="3" t="s">
         <v>35</v>
       </c>
@@ -8014,19 +8011,19 @@
         <v>66</v>
       </c>
       <c r="H129" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="I129" s="3" t="s">
         <v>640</v>
-      </c>
-      <c r="I129" s="3" t="s">
-        <v>641</v>
       </c>
       <c r="J129" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K129" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="L129" s="3" t="s">
         <v>642</v>
-      </c>
-      <c r="L129" s="3" t="s">
-        <v>643</v>
       </c>
       <c r="M129" s="3"/>
       <c r="N129" s="3"/>
@@ -8035,10 +8032,10 @@
       <c r="Q129" s="2"/>
     </row>
     <row r="130" spans="1:17" ht="15" customHeight="1">
-      <c r="A130" s="6" t="s">
-        <v>644</v>
-      </c>
-      <c r="B130" s="6"/>
+      <c r="A130" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="B130" s="8"/>
       <c r="C130" s="3" t="s">
         <v>58</v>
       </c>
@@ -8058,13 +8055,13 @@
         <v>207</v>
       </c>
       <c r="I130" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="J130" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="J130" s="3" t="s">
+      <c r="K130" s="3" t="s">
         <v>646</v>
-      </c>
-      <c r="K130" s="3" t="s">
-        <v>647</v>
       </c>
       <c r="L130" s="3" t="s">
         <v>261</v>
@@ -8076,10 +8073,10 @@
       <c r="Q130" s="2"/>
     </row>
     <row r="131" spans="1:17" ht="15" customHeight="1">
-      <c r="A131" s="6" t="s">
-        <v>648</v>
-      </c>
-      <c r="B131" s="6"/>
+      <c r="A131" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="B131" s="8"/>
       <c r="C131" s="3" t="s">
         <v>64</v>
       </c>
@@ -8096,19 +8093,19 @@
         <v>66</v>
       </c>
       <c r="H131" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="I131" s="3" t="s">
         <v>649</v>
-      </c>
-      <c r="I131" s="3" t="s">
-        <v>650</v>
       </c>
       <c r="J131" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K131" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="L131" s="3" t="s">
         <v>651</v>
-      </c>
-      <c r="L131" s="3" t="s">
-        <v>652</v>
       </c>
       <c r="M131" s="3"/>
       <c r="N131" s="3"/>
@@ -8117,10 +8114,10 @@
       <c r="Q131" s="2"/>
     </row>
     <row r="132" spans="1:17" ht="15" customHeight="1">
-      <c r="A132" s="6" t="s">
-        <v>653</v>
-      </c>
-      <c r="B132" s="6"/>
+      <c r="A132" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="B132" s="8"/>
       <c r="C132" s="3" t="s">
         <v>22</v>
       </c>
@@ -8140,16 +8137,16 @@
         <v>377</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J132" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K132" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="L132" s="3" t="s">
         <v>655</v>
-      </c>
-      <c r="L132" s="3" t="s">
-        <v>656</v>
       </c>
       <c r="M132" s="3"/>
       <c r="N132" s="3"/>
@@ -8158,10 +8155,10 @@
       <c r="Q132" s="2"/>
     </row>
     <row r="133" spans="1:17" ht="15" customHeight="1">
-      <c r="A133" s="6" t="s">
-        <v>657</v>
-      </c>
-      <c r="B133" s="6"/>
+      <c r="A133" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="B133" s="8"/>
       <c r="C133" s="3" t="s">
         <v>35</v>
       </c>
@@ -8178,19 +8175,19 @@
         <v>66</v>
       </c>
       <c r="H133" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="I133" s="3" t="s">
         <v>658</v>
-      </c>
-      <c r="I133" s="3" t="s">
-        <v>659</v>
       </c>
       <c r="J133" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K133" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="L133" s="3" t="s">
         <v>660</v>
-      </c>
-      <c r="L133" s="3" t="s">
-        <v>661</v>
       </c>
       <c r="M133" s="3"/>
       <c r="N133" s="3"/>
@@ -8199,10 +8196,10 @@
       <c r="Q133" s="2"/>
     </row>
     <row r="134" spans="1:17" ht="15" customHeight="1">
-      <c r="A134" s="6" t="s">
-        <v>662</v>
-      </c>
-      <c r="B134" s="6"/>
+      <c r="A134" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="B134" s="8"/>
       <c r="C134" s="3" t="s">
         <v>35</v>
       </c>
@@ -8219,19 +8216,19 @@
         <v>66</v>
       </c>
       <c r="H134" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="I134" s="3" t="s">
         <v>663</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>664</v>
       </c>
       <c r="J134" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K134" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="L134" s="3" t="s">
         <v>665</v>
-      </c>
-      <c r="L134" s="3" t="s">
-        <v>666</v>
       </c>
       <c r="M134" s="3"/>
       <c r="N134" s="3"/>
@@ -8240,10 +8237,10 @@
       <c r="Q134" s="2"/>
     </row>
     <row r="135" spans="1:17" ht="15" customHeight="1">
-      <c r="A135" s="6" t="s">
-        <v>667</v>
-      </c>
-      <c r="B135" s="6"/>
+      <c r="A135" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="B135" s="8"/>
       <c r="C135" s="3" t="s">
         <v>35</v>
       </c>
@@ -8260,19 +8257,19 @@
         <v>66</v>
       </c>
       <c r="H135" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="I135" s="3" t="s">
         <v>668</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>669</v>
       </c>
       <c r="J135" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K135" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="L135" s="3" t="s">
         <v>670</v>
-      </c>
-      <c r="L135" s="3" t="s">
-        <v>671</v>
       </c>
       <c r="M135" s="3"/>
       <c r="N135" s="3"/>
@@ -8281,10 +8278,10 @@
       <c r="Q135" s="2"/>
     </row>
     <row r="136" spans="1:17" ht="15" customHeight="1">
-      <c r="A136" s="6" t="s">
-        <v>672</v>
-      </c>
-      <c r="B136" s="6"/>
+      <c r="A136" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="B136" s="8"/>
       <c r="C136" s="3" t="s">
         <v>22</v>
       </c>
@@ -8301,19 +8298,19 @@
         <v>66</v>
       </c>
       <c r="H136" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="I136" s="3" t="s">
         <v>673</v>
-      </c>
-      <c r="I136" s="3" t="s">
-        <v>674</v>
       </c>
       <c r="J136" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K136" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="L136" s="3" t="s">
         <v>675</v>
-      </c>
-      <c r="L136" s="3" t="s">
-        <v>676</v>
       </c>
       <c r="M136" s="3"/>
       <c r="N136" s="3"/>
@@ -8322,10 +8319,10 @@
       <c r="Q136" s="2"/>
     </row>
     <row r="137" spans="1:17" ht="15" customHeight="1">
-      <c r="A137" s="6" t="s">
-        <v>677</v>
-      </c>
-      <c r="B137" s="6"/>
+      <c r="A137" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="B137" s="8"/>
       <c r="C137" s="3" t="s">
         <v>130</v>
       </c>
@@ -8342,19 +8339,19 @@
         <v>66</v>
       </c>
       <c r="H137" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="I137" s="3" t="s">
         <v>678</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>679</v>
       </c>
       <c r="J137" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K137" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="L137" s="3" t="s">
         <v>680</v>
-      </c>
-      <c r="L137" s="3" t="s">
-        <v>681</v>
       </c>
       <c r="M137" s="3"/>
       <c r="N137" s="3"/>
@@ -8363,10 +8360,10 @@
       <c r="Q137" s="2"/>
     </row>
     <row r="138" spans="1:17" ht="15" customHeight="1">
-      <c r="A138" s="6" t="s">
-        <v>682</v>
-      </c>
-      <c r="B138" s="6"/>
+      <c r="A138" s="8" t="s">
+        <v>681</v>
+      </c>
+      <c r="B138" s="8"/>
       <c r="C138" s="3" t="s">
         <v>64</v>
       </c>
@@ -8383,19 +8380,19 @@
         <v>66</v>
       </c>
       <c r="H138" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="I138" s="3" t="s">
         <v>683</v>
-      </c>
-      <c r="I138" s="3" t="s">
-        <v>684</v>
       </c>
       <c r="J138" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K138" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="L138" s="3" t="s">
         <v>685</v>
-      </c>
-      <c r="L138" s="3" t="s">
-        <v>686</v>
       </c>
       <c r="M138" s="3"/>
       <c r="N138" s="3"/>
@@ -8404,10 +8401,10 @@
       <c r="Q138" s="2"/>
     </row>
     <row r="139" spans="1:17" ht="15" customHeight="1">
-      <c r="A139" s="6" t="s">
-        <v>687</v>
-      </c>
-      <c r="B139" s="6"/>
+      <c r="A139" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="B139" s="8"/>
       <c r="C139" s="3" t="s">
         <v>22</v>
       </c>
@@ -8424,19 +8421,19 @@
         <v>66</v>
       </c>
       <c r="H139" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="I139" s="3" t="s">
         <v>688</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>689</v>
       </c>
       <c r="J139" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K139" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="L139" s="3" t="s">
         <v>690</v>
-      </c>
-      <c r="L139" s="3" t="s">
-        <v>691</v>
       </c>
       <c r="M139" s="3"/>
       <c r="N139" s="3"/>
@@ -8445,10 +8442,10 @@
       <c r="Q139" s="2"/>
     </row>
     <row r="140" spans="1:17" ht="15" customHeight="1">
-      <c r="A140" s="6" t="s">
-        <v>692</v>
-      </c>
-      <c r="B140" s="6"/>
+      <c r="A140" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="B140" s="8"/>
       <c r="C140" s="3" t="s">
         <v>35</v>
       </c>
@@ -8465,19 +8462,19 @@
         <v>66</v>
       </c>
       <c r="H140" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="I140" s="3" t="s">
         <v>693</v>
-      </c>
-      <c r="I140" s="3" t="s">
-        <v>694</v>
       </c>
       <c r="J140" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K140" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="L140" s="3" t="s">
         <v>695</v>
-      </c>
-      <c r="L140" s="3" t="s">
-        <v>696</v>
       </c>
       <c r="M140" s="3"/>
       <c r="N140" s="3"/>
@@ -8486,10 +8483,10 @@
       <c r="Q140" s="2"/>
     </row>
     <row r="141" spans="1:17" ht="15" customHeight="1">
-      <c r="A141" s="6" t="s">
-        <v>697</v>
-      </c>
-      <c r="B141" s="6"/>
+      <c r="A141" s="8" t="s">
+        <v>696</v>
+      </c>
+      <c r="B141" s="8"/>
       <c r="C141" s="3" t="s">
         <v>22</v>
       </c>
@@ -8506,19 +8503,19 @@
         <v>66</v>
       </c>
       <c r="H141" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="I141" s="3" t="s">
         <v>698</v>
-      </c>
-      <c r="I141" s="3" t="s">
-        <v>699</v>
       </c>
       <c r="J141" s="3" t="s">
         <v>224</v>
       </c>
       <c r="K141" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="L141" s="3" t="s">
         <v>700</v>
-      </c>
-      <c r="L141" s="3" t="s">
-        <v>701</v>
       </c>
       <c r="M141" s="3"/>
       <c r="N141" s="3"/>
@@ -8527,10 +8524,10 @@
       <c r="Q141" s="2"/>
     </row>
     <row r="142" spans="1:17" ht="15" customHeight="1">
-      <c r="A142" s="6" t="s">
-        <v>702</v>
-      </c>
-      <c r="B142" s="6"/>
+      <c r="A142" s="8" t="s">
+        <v>701</v>
+      </c>
+      <c r="B142" s="8"/>
       <c r="C142" s="3" t="s">
         <v>35</v>
       </c>
@@ -8544,22 +8541,22 @@
         <v>65</v>
       </c>
       <c r="G142" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="H142" s="3" t="s">
         <v>703</v>
       </c>
-      <c r="H142" s="3" t="s">
+      <c r="I142" s="3" t="s">
         <v>704</v>
-      </c>
-      <c r="I142" s="3" t="s">
-        <v>705</v>
       </c>
       <c r="J142" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K142" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="L142" s="3" t="s">
         <v>706</v>
-      </c>
-      <c r="L142" s="3" t="s">
-        <v>707</v>
       </c>
       <c r="M142" s="3"/>
       <c r="N142" s="3"/>
@@ -8568,10 +8565,10 @@
       <c r="Q142" s="2"/>
     </row>
     <row r="143" spans="1:17" ht="15" customHeight="1">
-      <c r="A143" s="6" t="s">
-        <v>708</v>
-      </c>
-      <c r="B143" s="6"/>
+      <c r="A143" s="8" t="s">
+        <v>707</v>
+      </c>
+      <c r="B143" s="8"/>
       <c r="C143" s="3" t="s">
         <v>35</v>
       </c>
@@ -8585,22 +8582,22 @@
         <v>65</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H143" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="I143" s="3" t="s">
         <v>709</v>
-      </c>
-      <c r="I143" s="3" t="s">
-        <v>710</v>
       </c>
       <c r="J143" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K143" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="L143" s="3" t="s">
         <v>711</v>
-      </c>
-      <c r="L143" s="3" t="s">
-        <v>712</v>
       </c>
       <c r="M143" s="3"/>
       <c r="N143" s="3"/>
@@ -8609,10 +8606,10 @@
       <c r="Q143" s="2"/>
     </row>
     <row r="144" spans="1:17" ht="15" customHeight="1">
-      <c r="A144" s="6" t="s">
-        <v>713</v>
-      </c>
-      <c r="B144" s="6"/>
+      <c r="A144" s="8" t="s">
+        <v>712</v>
+      </c>
+      <c r="B144" s="8"/>
       <c r="C144" s="3" t="s">
         <v>22</v>
       </c>
@@ -8626,22 +8623,22 @@
         <v>65</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H144" s="3" t="s">
+        <v>713</v>
+      </c>
+      <c r="I144" s="3" t="s">
         <v>714</v>
-      </c>
-      <c r="I144" s="3" t="s">
-        <v>715</v>
       </c>
       <c r="J144" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K144" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="L144" s="3" t="s">
         <v>716</v>
-      </c>
-      <c r="L144" s="3" t="s">
-        <v>717</v>
       </c>
       <c r="M144" s="3"/>
       <c r="N144" s="3"/>
@@ -8650,10 +8647,10 @@
       <c r="Q144" s="2"/>
     </row>
     <row r="145" spans="1:17" ht="15" customHeight="1">
-      <c r="A145" s="6" t="s">
-        <v>718</v>
-      </c>
-      <c r="B145" s="6"/>
+      <c r="A145" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B145" s="8"/>
       <c r="C145" s="3" t="s">
         <v>22</v>
       </c>
@@ -8667,22 +8664,22 @@
         <v>65</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H145" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="I145" s="3" t="s">
         <v>719</v>
-      </c>
-      <c r="I145" s="3" t="s">
-        <v>720</v>
       </c>
       <c r="J145" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K145" s="3" t="s">
+        <v>720</v>
+      </c>
+      <c r="L145" s="3" t="s">
         <v>721</v>
-      </c>
-      <c r="L145" s="3" t="s">
-        <v>722</v>
       </c>
       <c r="M145" s="3"/>
       <c r="N145" s="3"/>
@@ -8691,10 +8688,10 @@
       <c r="Q145" s="2"/>
     </row>
     <row r="146" spans="1:17" ht="15" customHeight="1">
-      <c r="A146" s="6" t="s">
-        <v>723</v>
-      </c>
-      <c r="B146" s="6"/>
+      <c r="A146" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="B146" s="8"/>
       <c r="C146" s="3" t="s">
         <v>58</v>
       </c>
@@ -8708,22 +8705,22 @@
         <v>73</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H146" s="3" t="s">
+        <v>723</v>
+      </c>
+      <c r="I146" s="3" t="s">
         <v>724</v>
-      </c>
-      <c r="I146" s="3" t="s">
-        <v>725</v>
       </c>
       <c r="J146" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K146" s="3" t="s">
+        <v>725</v>
+      </c>
+      <c r="L146" s="3" t="s">
         <v>726</v>
-      </c>
-      <c r="L146" s="3" t="s">
-        <v>727</v>
       </c>
       <c r="M146" s="3"/>
       <c r="N146" s="3"/>
@@ -8732,10 +8729,10 @@
       <c r="Q146" s="2"/>
     </row>
     <row r="147" spans="1:17" ht="15" customHeight="1">
-      <c r="A147" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="B147" s="6"/>
+      <c r="A147" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="B147" s="8"/>
       <c r="C147" s="3" t="s">
         <v>58</v>
       </c>
@@ -8749,19 +8746,19 @@
         <v>73</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H147" s="3" t="s">
+        <v>728</v>
+      </c>
+      <c r="I147" s="3" t="s">
         <v>729</v>
-      </c>
-      <c r="I147" s="3" t="s">
-        <v>730</v>
       </c>
       <c r="J147" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K147" s="3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="L147" s="3" t="s">
         <v>123</v>
@@ -8773,10 +8770,10 @@
       <c r="Q147" s="2"/>
     </row>
     <row r="148" spans="1:17" ht="15" customHeight="1">
-      <c r="A148" s="6" t="s">
-        <v>732</v>
-      </c>
-      <c r="B148" s="6"/>
+      <c r="A148" s="8" t="s">
+        <v>731</v>
+      </c>
+      <c r="B148" s="8"/>
       <c r="C148" s="3" t="s">
         <v>35</v>
       </c>
@@ -8790,22 +8787,22 @@
         <v>80</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H148" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="I148" s="3" t="s">
         <v>733</v>
-      </c>
-      <c r="I148" s="3" t="s">
-        <v>734</v>
       </c>
       <c r="J148" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K148" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="L148" s="3" t="s">
         <v>735</v>
-      </c>
-      <c r="L148" s="3" t="s">
-        <v>736</v>
       </c>
       <c r="M148" s="3"/>
       <c r="N148" s="3"/>
@@ -8814,10 +8811,10 @@
       <c r="Q148" s="2"/>
     </row>
     <row r="149" spans="1:17" ht="15" customHeight="1">
-      <c r="A149" s="6" t="s">
-        <v>737</v>
-      </c>
-      <c r="B149" s="6"/>
+      <c r="A149" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="B149" s="8"/>
       <c r="C149" s="3" t="s">
         <v>35</v>
       </c>
@@ -8831,22 +8828,22 @@
         <v>97</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H149" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I149" s="3" t="s">
         <v>738</v>
-      </c>
-      <c r="I149" s="3" t="s">
-        <v>739</v>
       </c>
       <c r="J149" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K149" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="L149" s="3" t="s">
         <v>740</v>
-      </c>
-      <c r="L149" s="3" t="s">
-        <v>741</v>
       </c>
       <c r="M149" s="3"/>
       <c r="N149" s="3"/>
@@ -8855,10 +8852,10 @@
       <c r="Q149" s="2"/>
     </row>
     <row r="150" spans="1:17" ht="15" customHeight="1">
-      <c r="A150" s="6" t="s">
-        <v>742</v>
-      </c>
-      <c r="B150" s="6"/>
+      <c r="A150" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="B150" s="8"/>
       <c r="C150" s="3" t="s">
         <v>22</v>
       </c>
@@ -8872,13 +8869,13 @@
         <v>65</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J150" s="3" t="s">
         <v>49</v>
@@ -8887,7 +8884,7 @@
         <v>73</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="M150" s="3"/>
       <c r="N150" s="3"/>
@@ -8896,10 +8893,10 @@
       <c r="Q150" s="2"/>
     </row>
     <row r="151" spans="1:17" ht="15" customHeight="1">
-      <c r="A151" s="6" t="s">
-        <v>744</v>
-      </c>
-      <c r="B151" s="6"/>
+      <c r="A151" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="B151" s="8"/>
       <c r="C151" s="3" t="s">
         <v>64</v>
       </c>
@@ -8913,13 +8910,13 @@
         <v>65</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H151" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J151" s="3" t="s">
         <v>49</v>
@@ -8928,7 +8925,7 @@
         <v>73</v>
       </c>
       <c r="L151" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M151" s="3"/>
       <c r="N151" s="3"/>
@@ -8937,10 +8934,10 @@
       <c r="Q151" s="2"/>
     </row>
     <row r="152" spans="1:17" ht="15" customHeight="1">
-      <c r="A152" s="6" t="s">
-        <v>745</v>
-      </c>
-      <c r="B152" s="6"/>
+      <c r="A152" s="8" t="s">
+        <v>744</v>
+      </c>
+      <c r="B152" s="8"/>
       <c r="C152" s="3" t="s">
         <v>64</v>
       </c>
@@ -8954,22 +8951,22 @@
         <v>65</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J152" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L152" s="3" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="M152" s="3"/>
       <c r="N152" s="3"/>
@@ -8978,10 +8975,10 @@
       <c r="Q152" s="2"/>
     </row>
     <row r="153" spans="1:17" ht="15" customHeight="1">
-      <c r="A153" s="6" t="s">
-        <v>747</v>
-      </c>
-      <c r="B153" s="6"/>
+      <c r="A153" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B153" s="8"/>
       <c r="C153" s="3" t="s">
         <v>35</v>
       </c>
@@ -8995,22 +8992,22 @@
         <v>80</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H153" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="I153" s="3" t="s">
         <v>748</v>
-      </c>
-      <c r="I153" s="3" t="s">
-        <v>749</v>
       </c>
       <c r="J153" s="3" t="s">
         <v>49</v>
       </c>
       <c r="K153" s="3" t="s">
+        <v>749</v>
+      </c>
+      <c r="L153" s="3" t="s">
         <v>750</v>
-      </c>
-      <c r="L153" s="3" t="s">
-        <v>751</v>
       </c>
       <c r="M153" s="3"/>
       <c r="N153" s="3"/>
@@ -9019,10 +9016,10 @@
       <c r="Q153" s="2"/>
     </row>
     <row r="154" spans="1:17" ht="15" customHeight="1">
-      <c r="A154" s="6" t="s">
-        <v>752</v>
-      </c>
-      <c r="B154" s="6"/>
+      <c r="A154" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="B154" s="8"/>
       <c r="C154" s="3" t="s">
         <v>35</v>
       </c>
@@ -9036,20 +9033,20 @@
         <v>38</v>
       </c>
       <c r="G154" s="3" t="s">
+        <v>752</v>
+      </c>
+      <c r="H154" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="H154" s="3" t="s">
+      <c r="I154" s="3" t="s">
         <v>754</v>
       </c>
-      <c r="I154" s="3" t="s">
+      <c r="J154" s="3" t="s">
         <v>755</v>
-      </c>
-      <c r="J154" s="3" t="s">
-        <v>756</v>
       </c>
       <c r="K154" s="3"/>
       <c r="L154" s="3" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="M154" s="3"/>
       <c r="N154" s="3"/>
@@ -9059,51 +9056,105 @@
     </row>
   </sheetData>
   <mergeCells count="154">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="C2:O2"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="C4:O4"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A6:Q6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A154:B154"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A147:B147"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A141:B141"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A140:B140"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A133:B133"/>
+    <mergeCell ref="A134:B134"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A125:B125"/>
+    <mergeCell ref="A116:B116"/>
+    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A53:B53"/>
@@ -9114,105 +9165,51 @@
     <mergeCell ref="A48:B48"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A122:B122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="A116:B116"/>
-    <mergeCell ref="A117:B117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A133:B133"/>
-    <mergeCell ref="A134:B134"/>
-    <mergeCell ref="A135:B135"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A127:B127"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="A141:B141"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A143:B143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A137:B137"/>
-    <mergeCell ref="A138:B138"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A140:B140"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A147:B147"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A6:Q6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="C2:O2"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="C4:O4"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>